<commit_message>
Added matched ifo evaluation
</commit_message>
<xml_diff>
--- a/1_Result_Tables/4_ifoCAST_evaluations_full/ifoCAst_error_tables_full_T45.xlsx
+++ b/1_Result_Tables/4_ifoCAST_evaluations_full/ifoCAst_error_tables_full_T45.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>ME</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>Q0</t>
+  </si>
+  <si>
+    <t>Q1</t>
   </si>
 </sst>
 </file>
@@ -395,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -426,22 +429,22 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>0.292290767741366</v>
+        <v>0.2247871045231402</v>
       </c>
       <c r="C2">
-        <v>2.028214721616381</v>
+        <v>2.035146975718185</v>
       </c>
       <c r="D2">
-        <v>17.22038356571953</v>
+        <v>17.83605474045861</v>
       </c>
       <c r="E2">
-        <v>4.149745000083684</v>
+        <v>4.223275356930757</v>
       </c>
       <c r="F2">
-        <v>4.154628978599494</v>
+        <v>4.269679570594401</v>
       </c>
       <c r="G2">
-        <v>137</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -449,22 +452,45 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>0.1627375324060313</v>
+        <v>0.2728254128479093</v>
       </c>
       <c r="C3">
-        <v>1.47175507077045</v>
+        <v>1.970770711136308</v>
       </c>
       <c r="D3">
-        <v>8.117450165288892</v>
+        <v>15.69395479060738</v>
       </c>
       <c r="E3">
-        <v>2.849113926344275</v>
+        <v>3.961559641177623</v>
       </c>
       <c r="F3">
-        <v>2.858237172666455</v>
+        <v>3.967096014706342</v>
       </c>
       <c r="G3">
-        <v>104</v>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>0.171141602336921</v>
+      </c>
+      <c r="C4">
+        <v>1.274244979641737</v>
+      </c>
+      <c r="D4">
+        <v>5.743778122149821</v>
+      </c>
+      <c r="E4">
+        <v>2.396618059297272</v>
+      </c>
+      <c r="F4">
+        <v>2.408541433280348</v>
+      </c>
+      <c r="G4">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>